<commit_message>
some updates to files for accurate data extraction
</commit_message>
<xml_diff>
--- a/Data Sets/Analysis Data/Community Profiles Compiled.xlsx
+++ b/Data Sets/Analysis Data/Community Profiles Compiled.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofc-my.sharepoint.com/personal/fahmid_kaisar_ucalgary_ca/Documents/Calgary Transit Repository/Data Sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sulemanbasit/PycharmProjects/Calgary-Transit-Economic-Gap-Analysis/Data Sets/Analysis Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4302" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BA701C8-00B3-4343-A32B-8786D088487A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C48A320-F284-EB47-B657-E0513531F019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="500" windowWidth="15420" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,9 +452,6 @@
     <t>Hillhurst</t>
   </si>
   <si>
-    <t>Hounsfeild Heights/Briar Hill</t>
-  </si>
-  <si>
     <t>Hungtington Hills</t>
   </si>
   <si>
@@ -798,6 +795,9 @@
   </si>
   <si>
     <t>Yorkville</t>
+  </si>
+  <si>
+    <t>Hounsfield Heights/Briar Hill</t>
   </si>
 </sst>
 </file>
@@ -1693,10 +1693,6 @@
 </externalLink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0554B52F-7523-4D92-8A4F-3A541CFE75ED}" name="Table1" displayName="Table1" ref="A1:AV268" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49" dataCellStyle="Comma">
   <autoFilter ref="A1:AV268" xr:uid="{0554B52F-7523-4D92-8A4F-3A541CFE75ED}"/>
@@ -2056,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15092,7 +15088,7 @@
     </row>
     <row r="90" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="B90" s="7">
         <v>2470</v>
@@ -15238,7 +15234,7 @@
     </row>
     <row r="91" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B91" s="7">
         <v>13120</v>
@@ -15301,7 +15297,7 @@
         <v>940</v>
       </c>
       <c r="V91" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W91" s="6">
         <v>220</v>
@@ -15384,7 +15380,7 @@
     </row>
     <row r="92" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B92" s="7">
         <v>4130</v>
@@ -15530,7 +15526,7 @@
     </row>
     <row r="93" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B93" s="7">
         <v>1805</v>
@@ -15676,7 +15672,7 @@
     </row>
     <row r="94" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B94" s="7">
         <v>7920</v>
@@ -15822,7 +15818,7 @@
     </row>
     <row r="95" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B95" s="7">
         <v>7030</v>
@@ -15968,7 +15964,7 @@
     </row>
     <row r="96" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B96" s="7">
         <v>4900</v>
@@ -16114,7 +16110,7 @@
     </row>
     <row r="97" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B97" s="7">
         <v>10145</v>
@@ -16260,7 +16256,7 @@
     </row>
     <row r="98" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B98" s="7">
         <v>5640</v>
@@ -16406,7 +16402,7 @@
     </row>
     <row r="99" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B99" s="7">
         <v>8100</v>
@@ -16552,7 +16548,7 @@
     </row>
     <row r="100" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B100" s="7">
         <v>1590</v>
@@ -16698,7 +16694,7 @@
     </row>
     <row r="101" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B101" s="7">
         <v>3985</v>
@@ -16844,7 +16840,7 @@
     </row>
     <row r="102" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102" s="7">
         <v>2990</v>
@@ -16990,7 +16986,7 @@
     </row>
     <row r="103" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B103" s="7">
         <v>4740</v>
@@ -17136,7 +17132,7 @@
     </row>
     <row r="104" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B104" s="7">
         <v>13860</v>
@@ -17282,7 +17278,7 @@
     </row>
     <row r="105" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B105" s="6">
         <v>950</v>
@@ -17428,7 +17424,7 @@
     </row>
     <row r="106" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B106" s="7">
         <v>1830</v>
@@ -17574,7 +17570,7 @@
     </row>
     <row r="107" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B107" s="7">
         <v>8910</v>
@@ -17720,7 +17716,7 @@
     </row>
     <row r="108" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B108" s="7">
         <v>14540</v>
@@ -17866,7 +17862,7 @@
     </row>
     <row r="109" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B109" s="6">
         <v>410</v>
@@ -18012,7 +18008,7 @@
     </row>
     <row r="110" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B110" s="7">
         <v>5925</v>
@@ -18158,7 +18154,7 @@
     </row>
     <row r="111" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B111" s="7">
         <v>13290</v>
@@ -18304,7 +18300,7 @@
     </row>
     <row r="112" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B112" s="7">
         <v>17505</v>
@@ -18450,7 +18446,7 @@
     </row>
     <row r="113" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B113" s="6">
         <v>610</v>
@@ -18596,7 +18592,7 @@
     </row>
     <row r="114" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B114" s="7">
         <v>6480</v>
@@ -18742,7 +18738,7 @@
     </row>
     <row r="115" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B115" s="7">
         <v>6655</v>
@@ -18888,7 +18884,7 @@
     </row>
     <row r="116" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B116" s="7">
         <v>4505</v>
@@ -19034,7 +19030,7 @@
     </row>
     <row r="117" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A117" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B117" s="7">
         <v>10475</v>
@@ -19180,7 +19176,7 @@
     </row>
     <row r="118" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B118" s="7">
         <v>4175</v>
@@ -19326,7 +19322,7 @@
     </row>
     <row r="119" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B119" s="7">
         <v>6325</v>
@@ -19472,7 +19468,7 @@
     </row>
     <row r="120" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A120" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B120" s="7">
         <v>12885</v>
@@ -19618,7 +19614,7 @@
     </row>
     <row r="121" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A121" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B121" s="7">
         <v>8755</v>
@@ -19764,7 +19760,7 @@
     </row>
     <row r="122" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A122" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B122" s="7">
         <v>2435</v>
@@ -19910,7 +19906,7 @@
     </row>
     <row r="123" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A123" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B123" s="7">
         <v>2365</v>
@@ -20056,7 +20052,7 @@
     </row>
     <row r="124" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A124" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B124" s="9">
         <v>640</v>
@@ -20202,7 +20198,7 @@
     </row>
     <row r="125" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B125" s="9">
         <v>5620</v>
@@ -20348,7 +20344,7 @@
     </row>
     <row r="126" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A126" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B126" s="9">
         <v>8315</v>
@@ -20494,7 +20490,7 @@
     </row>
     <row r="127" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B127" s="9">
         <v>3285</v>
@@ -20640,7 +20636,7 @@
     </row>
     <row r="128" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A128" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B128" s="9">
         <v>25535</v>
@@ -20786,7 +20782,7 @@
     </row>
     <row r="129" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B129" s="9">
         <v>2300</v>
@@ -20932,7 +20928,7 @@
     </row>
     <row r="130" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A130" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B130" s="9">
         <v>1770</v>
@@ -21078,7 +21074,7 @@
     </row>
     <row r="131" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B131" s="9">
         <v>3430</v>
@@ -21224,7 +21220,7 @@
     </row>
     <row r="132" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A132" s="9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B132" s="9">
         <v>4145</v>
@@ -21370,7 +21366,7 @@
     </row>
     <row r="133" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A133" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B133" s="9">
         <v>8235</v>
@@ -21516,7 +21512,7 @@
     </row>
     <row r="134" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B134" s="9">
         <v>245</v>
@@ -21552,43 +21548,43 @@
         <v>98000</v>
       </c>
       <c r="M134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="O134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Q134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="S134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="T134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="W134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="X134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Y134" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z134" s="12">
         <v>85</v>
@@ -21597,10 +21593,10 @@
         <v>0</v>
       </c>
       <c r="AB134" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AC134" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AD134" s="9">
         <v>85</v>
@@ -21662,7 +21658,7 @@
     </row>
     <row r="135" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B135" s="9">
         <v>9850</v>
@@ -21808,7 +21804,7 @@
     </row>
     <row r="136" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A136" s="9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B136" s="9">
         <v>1330</v>
@@ -21954,7 +21950,7 @@
     </row>
     <row r="137" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A137" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B137" s="9">
         <v>1455</v>
@@ -22100,7 +22096,7 @@
     </row>
     <row r="138" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A138" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B138" s="9">
         <v>375</v>
@@ -22246,7 +22242,7 @@
     </row>
     <row r="139" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B139" s="9">
         <v>4585</v>
@@ -22392,7 +22388,7 @@
     </row>
     <row r="140" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A140" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B140" s="9">
         <v>2155</v>
@@ -22538,7 +22534,7 @@
     </row>
     <row r="141" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B141" s="9">
         <v>7490</v>
@@ -22684,7 +22680,7 @@
     </row>
     <row r="142" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A142" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B142" s="9">
         <v>1745</v>
@@ -22830,7 +22826,7 @@
     </row>
     <row r="143" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A143" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B143" s="9">
         <v>9050</v>
@@ -22976,7 +22972,7 @@
     </row>
     <row r="144" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B144" s="9">
         <v>6580</v>
@@ -23122,7 +23118,7 @@
     </row>
     <row r="145" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A145" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B145" s="9">
         <v>5250</v>
@@ -23268,7 +23264,7 @@
     </row>
     <row r="146" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A146" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B146" s="9">
         <v>675</v>
@@ -23414,7 +23410,7 @@
     </row>
     <row r="147" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A147" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B147" s="9">
         <v>9205</v>
@@ -23560,7 +23556,7 @@
     </row>
     <row r="148" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A148" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B148" s="9">
         <v>8195</v>
@@ -23706,7 +23702,7 @@
     </row>
     <row r="149" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B149" s="9">
         <v>1495</v>
@@ -23852,7 +23848,7 @@
     </row>
     <row r="150" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A150" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B150" s="9">
         <v>1155</v>
@@ -23998,7 +23994,7 @@
     </row>
     <row r="151" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A151" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B151" s="9">
         <v>3490</v>
@@ -24144,7 +24140,7 @@
     </row>
     <row r="152" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A152" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B152" s="9">
         <v>415</v>
@@ -24290,7 +24286,7 @@
     </row>
     <row r="153" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A153" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B153" s="9">
         <v>11580</v>
@@ -24436,7 +24432,7 @@
     </row>
     <row r="154" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A154" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B154" s="9">
         <v>10545</v>
@@ -24582,7 +24578,7 @@
     </row>
     <row r="155" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A155" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B155" s="9">
         <v>2140</v>
@@ -24728,7 +24724,7 @@
     </row>
     <row r="156" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A156" s="9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B156" s="9">
         <v>24365</v>
@@ -24874,7 +24870,7 @@
     </row>
     <row r="157" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A157" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B157" s="9">
         <v>9345</v>
@@ -25020,7 +25016,7 @@
     </row>
     <row r="158" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A158" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B158" s="9">
         <v>5795</v>
@@ -25166,7 +25162,7 @@
     </row>
     <row r="159" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A159" s="9" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B159" s="9">
         <v>1010</v>
@@ -25312,7 +25308,7 @@
     </row>
     <row r="160" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A160" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B160" s="9">
         <v>465</v>
@@ -25458,7 +25454,7 @@
     </row>
     <row r="161" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A161" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B161" s="9">
         <v>7850</v>
@@ -25604,7 +25600,7 @@
     </row>
     <row r="162" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A162" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B162" s="9">
         <v>3590</v>
@@ -25750,7 +25746,7 @@
     </row>
     <row r="163" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B163" s="9">
         <v>1765</v>
@@ -25896,7 +25892,7 @@
     </row>
     <row r="164" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A164" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B164" s="9">
         <v>2020</v>
@@ -26042,7 +26038,7 @@
     </row>
     <row r="165" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A165" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B165" s="9">
         <v>9055</v>
@@ -26188,7 +26184,7 @@
     </row>
     <row r="166" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A166" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B166" s="9">
         <v>265</v>
@@ -26335,7 +26331,7 @@
     </row>
     <row r="167" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A167" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B167" s="9">
         <v>6520</v>
@@ -26482,7 +26478,7 @@
     </row>
     <row r="168" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B168" s="9">
         <v>13000</v>
@@ -26629,7 +26625,7 @@
     </row>
     <row r="169" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A169" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B169" s="9">
         <v>8570</v>
@@ -26776,7 +26772,7 @@
     </row>
     <row r="170" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A170" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B170" s="9">
         <v>12870</v>
@@ -26924,7 +26920,7 @@
     </row>
     <row r="171" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A171" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B171" s="9">
         <v>8320</v>
@@ -27070,7 +27066,7 @@
     </row>
     <row r="172" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A172" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B172" s="9">
         <v>4540</v>
@@ -27216,7 +27212,7 @@
     </row>
     <row r="173" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B173" s="9">
         <v>1550</v>
@@ -27362,7 +27358,7 @@
     </row>
     <row r="174" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A174" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B174" s="9">
         <v>6095</v>
@@ -27508,7 +27504,7 @@
     </row>
     <row r="175" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A175" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B175" s="9">
         <v>9840</v>
@@ -27654,7 +27650,7 @@
     </row>
     <row r="176" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A176" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B176" s="9">
         <v>4195</v>
@@ -27800,7 +27796,7 @@
     </row>
     <row r="177" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A177" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B177" s="9">
         <v>1345</v>
@@ -27946,7 +27942,7 @@
     </row>
     <row r="178" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A178" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B178" s="9">
         <v>6830</v>
@@ -28092,7 +28088,7 @@
     </row>
     <row r="179" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A179" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B179" s="9">
         <v>9590</v>
@@ -28238,7 +28234,7 @@
     </row>
     <row r="180" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A180" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B180" s="9">
         <v>4000</v>
@@ -28384,7 +28380,7 @@
     </row>
     <row r="181" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A181" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B181" s="9">
         <v>3090</v>
@@ -28530,7 +28526,7 @@
     </row>
     <row r="182" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A182" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B182" s="9">
         <v>17630</v>
@@ -28676,7 +28672,7 @@
     </row>
     <row r="183" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A183" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B183" s="9">
         <v>10525</v>
@@ -28822,7 +28818,7 @@
     </row>
     <row r="184" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A184" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B184" s="9">
         <v>8695</v>
@@ -28968,7 +28964,7 @@
     </row>
     <row r="185" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A185" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B185" s="9">
         <v>19700</v>
@@ -29114,7 +29110,7 @@
     </row>
     <row r="186" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A186" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B186" s="9">
         <v>5165</v>
@@ -29260,7 +29256,7 @@
     </row>
     <row r="187" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A187" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B187" s="9">
         <v>2965</v>
@@ -29406,7 +29402,7 @@
     </row>
     <row r="188" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A188" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B188" s="9">
         <v>2735</v>
@@ -29552,7 +29548,7 @@
     </row>
     <row r="189" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A189" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B189" s="9">
         <v>5365</v>
@@ -29698,7 +29694,7 @@
     </row>
     <row r="190" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A190" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B190" s="9">
         <v>12040</v>
@@ -29844,7 +29840,7 @@
     </row>
     <row r="191" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A191" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B191" s="9">
         <v>7650</v>
@@ -29990,7 +29986,7 @@
     </row>
     <row r="192" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A192" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B192" s="9">
         <v>6635</v>
@@ -30136,7 +30132,7 @@
     </row>
     <row r="193" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A193" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B193" s="9">
         <v>11560</v>
@@ -30282,7 +30278,7 @@
     </row>
     <row r="194" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A194" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B194" s="9">
         <v>3225</v>
@@ -30428,7 +30424,7 @@
     </row>
     <row r="195" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A195" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B195" s="9">
         <v>11085</v>
@@ -30574,7 +30570,7 @@
     </row>
     <row r="196" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A196" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B196" s="9">
         <v>2765</v>
@@ -30720,7 +30716,7 @@
     </row>
     <row r="197" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A197" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B197" s="9">
         <v>5090</v>
@@ -30866,7 +30862,7 @@
     </row>
     <row r="198" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A198" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B198" s="9">
         <v>4410</v>
@@ -31012,7 +31008,7 @@
     </row>
     <row r="199" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A199" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B199" s="9">
         <v>3605</v>
@@ -31158,7 +31154,7 @@
     </row>
     <row r="200" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A200" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B200" s="9">
         <v>525</v>
@@ -31304,7 +31300,7 @@
     </row>
     <row r="201" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A201" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B201" s="9">
         <v>8745</v>
@@ -31450,7 +31446,7 @@
     </row>
     <row r="202" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A202" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B202" s="9">
         <v>5830</v>
@@ -31596,7 +31592,7 @@
     </row>
     <row r="203" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A203" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B203" s="9">
         <v>715</v>

</xml_diff>